<commit_message>
10 Feb 2020 Beep and Message Box
</commit_message>
<xml_diff>
--- a/realEstateData.xlsx
+++ b/realEstateData.xlsx
@@ -14,14 +14,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="171">
   <si>
     <t>POA</t>
   </si>
   <si>
-    <t>297 m²</t>
-  </si>
-  <si>
     <t>Cape Town City Centre</t>
   </si>
   <si>
@@ -40,9 +37,6 @@
     <t>43 m²</t>
   </si>
   <si>
-    <t>R 1 450 000</t>
-  </si>
-  <si>
     <t>R 1 495 000</t>
   </si>
   <si>
@@ -52,9 +46,6 @@
     <t>R 1 550 000</t>
   </si>
   <si>
-    <t>55 m²</t>
-  </si>
-  <si>
     <t>R 1 590 000</t>
   </si>
   <si>
@@ -64,15 +55,6 @@
     <t>50 m²</t>
   </si>
   <si>
-    <t>R 1 630 000</t>
-  </si>
-  <si>
-    <t>47 m²</t>
-  </si>
-  <si>
-    <t>R 1 650 000</t>
-  </si>
-  <si>
     <t>51 m²</t>
   </si>
   <si>
@@ -85,15 +67,9 @@
     <t>66 m²</t>
   </si>
   <si>
-    <t>R 1 800 000</t>
-  </si>
-  <si>
     <t>61 m²</t>
   </si>
   <si>
-    <t>R 1 850 000</t>
-  </si>
-  <si>
     <t>72 m²</t>
   </si>
   <si>
@@ -103,87 +79,27 @@
     <t>41 m²</t>
   </si>
   <si>
-    <t>64 m²</t>
-  </si>
-  <si>
     <t>R 10 500 000</t>
   </si>
   <si>
-    <t>170 m²</t>
-  </si>
-  <si>
-    <t>R 11 750 000</t>
-  </si>
-  <si>
-    <t>354 m²</t>
-  </si>
-  <si>
-    <t>R 12 250 000</t>
-  </si>
-  <si>
-    <t>349 m²</t>
-  </si>
-  <si>
-    <t>R 13 500 000</t>
-  </si>
-  <si>
     <t>230 m²</t>
   </si>
   <si>
-    <t>R 2 095 000</t>
-  </si>
-  <si>
-    <t>45 m²</t>
-  </si>
-  <si>
-    <t>R 2 199 000</t>
-  </si>
-  <si>
     <t>R 2 200 000</t>
   </si>
   <si>
-    <t>R 2 275 000</t>
-  </si>
-  <si>
-    <t>36 m²</t>
-  </si>
-  <si>
-    <t>R 2 300 000</t>
-  </si>
-  <si>
-    <t>132 m²</t>
-  </si>
-  <si>
-    <t>R 2 400 000</t>
-  </si>
-  <si>
     <t>83 m²</t>
   </si>
   <si>
-    <t>R 2 495 000</t>
-  </si>
-  <si>
     <t>71 m²</t>
   </si>
   <si>
-    <t>R 2 599 000</t>
-  </si>
-  <si>
-    <t>R 2 695 000</t>
-  </si>
-  <si>
     <t>85 m²</t>
   </si>
   <si>
-    <t>R 2 720 000</t>
-  </si>
-  <si>
     <t>58 m²</t>
   </si>
   <si>
-    <t>R 2 749 000</t>
-  </si>
-  <si>
     <t>R 2 750 000</t>
   </si>
   <si>
@@ -193,12 +109,6 @@
     <t>R 2 800 000</t>
   </si>
   <si>
-    <t>R 2 850 000</t>
-  </si>
-  <si>
-    <t>R 2 900 000</t>
-  </si>
-  <si>
     <t>R 2 950 000</t>
   </si>
   <si>
@@ -211,18 +121,9 @@
     <t>93 m²</t>
   </si>
   <si>
-    <t>110 m²</t>
-  </si>
-  <si>
-    <t>R 2 999 000</t>
-  </si>
-  <si>
     <t>59 m²</t>
   </si>
   <si>
-    <t>R 3 195 000</t>
-  </si>
-  <si>
     <t>128 m²</t>
   </si>
   <si>
@@ -235,9 +136,6 @@
     <t>R 3 295 000</t>
   </si>
   <si>
-    <t>R 3 395 000</t>
-  </si>
-  <si>
     <t>100 m²</t>
   </si>
   <si>
@@ -247,72 +145,9 @@
     <t>130 m²</t>
   </si>
   <si>
-    <t>R 3 495 000</t>
-  </si>
-  <si>
-    <t>125 m²</t>
-  </si>
-  <si>
-    <t>R 3 650 000</t>
-  </si>
-  <si>
     <t>87 m²</t>
   </si>
   <si>
-    <t>R 4 200 000</t>
-  </si>
-  <si>
-    <t>149 m²</t>
-  </si>
-  <si>
-    <t>R 4 250 000</t>
-  </si>
-  <si>
-    <t>143 m²</t>
-  </si>
-  <si>
-    <t>R 4 500 000</t>
-  </si>
-  <si>
-    <t>108 m²</t>
-  </si>
-  <si>
-    <t>R 4 750 000</t>
-  </si>
-  <si>
-    <t>109 m²</t>
-  </si>
-  <si>
-    <t>R 5 000 000</t>
-  </si>
-  <si>
-    <t>R 5 425 000</t>
-  </si>
-  <si>
-    <t>R 5 450 000</t>
-  </si>
-  <si>
-    <t>154 m²</t>
-  </si>
-  <si>
-    <t>R 5 850 000</t>
-  </si>
-  <si>
-    <t>84 m²</t>
-  </si>
-  <si>
-    <t>R 9 500 000</t>
-  </si>
-  <si>
-    <t>274 m²</t>
-  </si>
-  <si>
-    <t>R 9 975 000</t>
-  </si>
-  <si>
-    <t>171 m²</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
@@ -328,46 +163,370 @@
     <t>Location</t>
   </si>
   <si>
-    <t>R 1 874 500</t>
-  </si>
-  <si>
-    <t>R 2 050 000</t>
-  </si>
-  <si>
-    <t>R 1 350 000</t>
-  </si>
-  <si>
-    <t>52 m²</t>
-  </si>
-  <si>
-    <t>R 1 950 000</t>
-  </si>
-  <si>
-    <t>40 m²</t>
-  </si>
-  <si>
-    <t>R 2 070 000</t>
-  </si>
-  <si>
-    <t>R 2 150 000</t>
-  </si>
-  <si>
     <t>68 m²</t>
   </si>
   <si>
-    <t>R 2 180 000</t>
-  </si>
-  <si>
     <t>62 m²</t>
   </si>
   <si>
     <t>R 2 450 000</t>
   </si>
   <si>
-    <t>91 m²</t>
-  </si>
-  <si>
     <t>R 2 795 000</t>
+  </si>
+  <si>
+    <t>600 m²</t>
+  </si>
+  <si>
+    <t>Oranjezicht</t>
+  </si>
+  <si>
+    <t>42 m²</t>
+  </si>
+  <si>
+    <t>Claremont Upper</t>
+  </si>
+  <si>
+    <t>R 1 195 000</t>
+  </si>
+  <si>
+    <t>Plumstead</t>
+  </si>
+  <si>
+    <t>Mowbray</t>
+  </si>
+  <si>
+    <t>R 1 250 000</t>
+  </si>
+  <si>
+    <t>R 1 295 000</t>
+  </si>
+  <si>
+    <t>103 m²</t>
+  </si>
+  <si>
+    <t>Elfindale</t>
+  </si>
+  <si>
+    <t>Kenilworth</t>
+  </si>
+  <si>
+    <t>R 1 400 000</t>
+  </si>
+  <si>
+    <t>Woodstock</t>
+  </si>
+  <si>
+    <t>R 1 425 000</t>
+  </si>
+  <si>
+    <t>82 m²</t>
+  </si>
+  <si>
+    <t>R 1 475 000</t>
+  </si>
+  <si>
+    <t>Observatory</t>
+  </si>
+  <si>
+    <t>46 m²</t>
+  </si>
+  <si>
+    <t>Rondebosch</t>
+  </si>
+  <si>
+    <t>R 1 530 000</t>
+  </si>
+  <si>
+    <t>86 m²</t>
+  </si>
+  <si>
+    <t>30 m²</t>
+  </si>
+  <si>
+    <t>R 1 625 000</t>
+  </si>
+  <si>
+    <t>88 m²</t>
+  </si>
+  <si>
+    <t>R 1 695 000</t>
+  </si>
+  <si>
+    <t>65 m²</t>
+  </si>
+  <si>
+    <t>Zonnebloem</t>
+  </si>
+  <si>
+    <t>Gardens</t>
+  </si>
+  <si>
+    <t>R 1 999 000</t>
+  </si>
+  <si>
+    <t>121 m²</t>
+  </si>
+  <si>
+    <t>Green Point</t>
+  </si>
+  <si>
+    <t>R 10 995 000</t>
+  </si>
+  <si>
+    <t>Waterfront</t>
+  </si>
+  <si>
+    <t>R 14 990 000</t>
+  </si>
+  <si>
+    <t>135 m²</t>
+  </si>
+  <si>
+    <t>Clifton</t>
+  </si>
+  <si>
+    <t>R 15 700 000</t>
+  </si>
+  <si>
+    <t>188 m²</t>
+  </si>
+  <si>
+    <t>Sea Point</t>
+  </si>
+  <si>
+    <t>R 15 950 000</t>
+  </si>
+  <si>
+    <t>226 m²</t>
+  </si>
+  <si>
+    <t>Mouille Point</t>
+  </si>
+  <si>
+    <t>R 16 175 000</t>
+  </si>
+  <si>
+    <t>228 m²</t>
+  </si>
+  <si>
+    <t>R 16 850 000</t>
+  </si>
+  <si>
+    <t>206 m²</t>
+  </si>
+  <si>
+    <t>Camps Bay</t>
+  </si>
+  <si>
+    <t>R 18 950 000</t>
+  </si>
+  <si>
+    <t>320 m²</t>
+  </si>
+  <si>
+    <t>Fresnaye</t>
+  </si>
+  <si>
+    <t>R 2 195 000</t>
+  </si>
+  <si>
+    <t>Tamboerskloof</t>
+  </si>
+  <si>
+    <t>Wynberg Upper</t>
+  </si>
+  <si>
+    <t>R 2 395 000</t>
+  </si>
+  <si>
+    <t>90 m²</t>
+  </si>
+  <si>
+    <t>R 2 530 000</t>
+  </si>
+  <si>
+    <t>95 m²</t>
+  </si>
+  <si>
+    <t>Claremont</t>
+  </si>
+  <si>
+    <t>R 2 595 000</t>
+  </si>
+  <si>
+    <t>Kenilworth Upper</t>
+  </si>
+  <si>
+    <t>R 2 675 000</t>
+  </si>
+  <si>
+    <t>78 m²</t>
+  </si>
+  <si>
+    <t>74 m²</t>
+  </si>
+  <si>
+    <t>Three Anchor Bay</t>
+  </si>
+  <si>
+    <t>Vredehoek</t>
+  </si>
+  <si>
+    <t>75 m²</t>
+  </si>
+  <si>
+    <t>De Waterkant</t>
+  </si>
+  <si>
+    <t>105 m²</t>
+  </si>
+  <si>
+    <t>R 20 000 000</t>
+  </si>
+  <si>
+    <t>277 m²</t>
+  </si>
+  <si>
+    <t>R 20 995 000</t>
+  </si>
+  <si>
+    <t>225 m²</t>
+  </si>
+  <si>
+    <t>R 25 000 000</t>
+  </si>
+  <si>
+    <t>403 m²</t>
+  </si>
+  <si>
+    <t>R 3 149 000</t>
+  </si>
+  <si>
+    <t>76 m²</t>
+  </si>
+  <si>
+    <t>R 3 150 000</t>
+  </si>
+  <si>
+    <t>R 3 250 000</t>
+  </si>
+  <si>
+    <t>97 m²</t>
+  </si>
+  <si>
+    <t>R 3 275 000</t>
+  </si>
+  <si>
+    <t>81 m²</t>
+  </si>
+  <si>
+    <t>Foreshore</t>
+  </si>
+  <si>
+    <t>R 3 500 000</t>
+  </si>
+  <si>
+    <t>Kalk Bay</t>
+  </si>
+  <si>
+    <t>R 3 590 000</t>
+  </si>
+  <si>
+    <t>R 3 600 000</t>
+  </si>
+  <si>
+    <t>98 m²</t>
+  </si>
+  <si>
+    <t>R 3 750 000</t>
+  </si>
+  <si>
+    <t>R 3 850 000</t>
+  </si>
+  <si>
+    <t>R 3 945 000</t>
+  </si>
+  <si>
+    <t>169 m²</t>
+  </si>
+  <si>
+    <t>R 3 995 000</t>
+  </si>
+  <si>
+    <t>R 4 488 000</t>
+  </si>
+  <si>
+    <t>R 4 700 000</t>
+  </si>
+  <si>
+    <t>126 m²</t>
+  </si>
+  <si>
+    <t>R 5 300 000</t>
+  </si>
+  <si>
+    <t>80 m²</t>
+  </si>
+  <si>
+    <t>R 5 500 000</t>
+  </si>
+  <si>
+    <t>117 m²</t>
+  </si>
+  <si>
+    <t>R 5 700 000</t>
+  </si>
+  <si>
+    <t>178 m²</t>
+  </si>
+  <si>
+    <t>R 5 950 000</t>
+  </si>
+  <si>
+    <t>158 m²</t>
+  </si>
+  <si>
+    <t>R 7 250 000</t>
+  </si>
+  <si>
+    <t>136 m²</t>
+  </si>
+  <si>
+    <t>R 7 450 000</t>
+  </si>
+  <si>
+    <t>180 m²</t>
+  </si>
+  <si>
+    <t>R 7 750 000</t>
+  </si>
+  <si>
+    <t>211 m²</t>
+  </si>
+  <si>
+    <t>174 m²</t>
+  </si>
+  <si>
+    <t>R 8 450 000</t>
+  </si>
+  <si>
+    <t>157 m²</t>
+  </si>
+  <si>
+    <t>R 8 950 000</t>
+  </si>
+  <si>
+    <t>198 m²</t>
+  </si>
+  <si>
+    <t>R 850 000</t>
+  </si>
+  <si>
+    <t>Southfield</t>
+  </si>
+  <si>
+    <t>R 899 000</t>
   </si>
 </sst>
 </file>
@@ -706,7 +865,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E78"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -714,19 +873,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>102</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -734,106 +893,106 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="B5">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>61</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -842,15 +1001,15 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B9">
         <v>0.5</v>
@@ -859,66 +1018,66 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="B11">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="B12">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="E12" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -927,15 +1086,15 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="E13" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -944,15 +1103,15 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -961,32 +1120,32 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -995,49 +1154,49 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B19">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="E19" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1046,66 +1205,66 @@
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="E21" t="s">
-        <v>2</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>78</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>79</v>
       </c>
       <c r="E22" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="E23" t="s">
-        <v>2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>104</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1114,49 +1273,49 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="E24" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B25">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="E25" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1165,32 +1324,32 @@
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>109</v>
+        <v>55</v>
       </c>
       <c r="E27" t="s">
-        <v>2</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>21</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D28" t="s">
-        <v>109</v>
+        <v>83</v>
       </c>
       <c r="E28" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="B29">
         <v>2</v>
@@ -1199,134 +1358,134 @@
         <v>2</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E29" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E30" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>87</v>
       </c>
       <c r="B31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C31">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="E31" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="B32">
         <v>3</v>
       </c>
       <c r="C32">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="D32" t="s">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="E32" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="B33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C33">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="D33" t="s">
-        <v>39</v>
+        <v>94</v>
       </c>
       <c r="E33" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="D34" t="s">
-        <v>24</v>
+        <v>97</v>
       </c>
       <c r="E34" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="D35" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="E35" t="s">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C36">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="D36" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="E36" t="s">
-        <v>2</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1335,15 +1494,15 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>114</v>
+        <v>12</v>
       </c>
       <c r="E37" t="s">
-        <v>2</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1352,219 +1511,219 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="E38" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="E39" t="s">
-        <v>2</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B40">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>43</v>
+        <v>6</v>
       </c>
       <c r="E40" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>44</v>
+        <v>107</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E41" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="E42" t="s">
-        <v>2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="E43" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="E44" t="s">
-        <v>2</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>109</v>
       </c>
       <c r="B45">
         <v>2</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D45" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="E45" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="B46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C46">
         <v>2</v>
       </c>
       <c r="D46" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E46" t="s">
-        <v>2</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="B47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="E47" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48">
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>24</v>
+        <v>116</v>
       </c>
       <c r="E48" t="s">
-        <v>2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>28</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C49">
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>57</v>
+        <v>32</v>
       </c>
       <c r="E49" t="s">
-        <v>2</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>52</v>
       </c>
       <c r="B50">
         <v>2</v>
       </c>
       <c r="C50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="E50" t="s">
-        <v>2</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B51">
         <v>2</v>
@@ -1576,29 +1735,29 @@
         <v>24</v>
       </c>
       <c r="E51" t="s">
-        <v>2</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B52">
         <v>2</v>
       </c>
       <c r="C52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D52" t="s">
-        <v>24</v>
+        <v>119</v>
       </c>
       <c r="E52" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -1607,134 +1766,134 @@
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E53" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="E54" t="s">
-        <v>2</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C55">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D55" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="E55" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>122</v>
       </c>
       <c r="B56">
         <v>2</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="E56" t="s">
-        <v>2</v>
+        <v>103</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C57">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D57" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="E57" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C58">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D58" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="E58" t="s">
-        <v>2</v>
+        <v>100</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>70</v>
+        <v>128</v>
       </c>
       <c r="B59">
         <v>2</v>
       </c>
       <c r="C59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>71</v>
+        <v>129</v>
       </c>
       <c r="E59" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>130</v>
       </c>
       <c r="B60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C60">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>71</v>
+        <v>119</v>
       </c>
       <c r="E60" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>72</v>
+        <v>130</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -1743,32 +1902,32 @@
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="E61" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="B62">
         <v>2</v>
       </c>
       <c r="C62">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="E62" t="s">
-        <v>2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>75</v>
+        <v>37</v>
       </c>
       <c r="B63">
         <v>2</v>
@@ -1777,117 +1936,117 @@
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>76</v>
+        <v>40</v>
       </c>
       <c r="E63" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C64">
         <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>78</v>
+        <v>132</v>
       </c>
       <c r="E64" t="s">
-        <v>2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="B65">
         <v>2</v>
       </c>
       <c r="C65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>80</v>
+        <v>134</v>
       </c>
       <c r="E65" t="s">
-        <v>2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="B66">
         <v>2</v>
       </c>
       <c r="C66">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="E66" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>81</v>
+        <v>41</v>
       </c>
       <c r="B67">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
       <c r="D67" t="s">
-        <v>82</v>
+        <v>108</v>
       </c>
       <c r="E67" t="s">
-        <v>2</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="B68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C68">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D68" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="E68" t="s">
-        <v>2</v>
+        <v>135</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>83</v>
+        <v>136</v>
       </c>
       <c r="B69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C69">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D69" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="E69" t="s">
-        <v>2</v>
+        <v>137</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>85</v>
+        <v>138</v>
       </c>
       <c r="B70">
         <v>2</v>
@@ -1896,32 +2055,32 @@
         <v>2</v>
       </c>
       <c r="D70" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="E70" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>87</v>
+        <v>139</v>
       </c>
       <c r="B71">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C71">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>88</v>
+        <v>140</v>
       </c>
       <c r="E71" t="s">
-        <v>2</v>
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="B72">
         <v>2</v>
@@ -1930,15 +2089,15 @@
         <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="E72" t="s">
-        <v>2</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>90</v>
+        <v>142</v>
       </c>
       <c r="B73">
         <v>2</v>
@@ -1947,95 +2106,333 @@
         <v>2</v>
       </c>
       <c r="D73" t="s">
-        <v>65</v>
+        <v>24</v>
       </c>
       <c r="E73" t="s">
-        <v>2</v>
+        <v>118</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>91</v>
+        <v>143</v>
       </c>
       <c r="B74">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C74">
         <v>2</v>
       </c>
       <c r="D74" t="s">
-        <v>92</v>
+        <v>144</v>
       </c>
       <c r="E74" t="s">
-        <v>2</v>
+        <v>58</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C75">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D75" t="s">
-        <v>94</v>
+        <v>140</v>
       </c>
       <c r="E75" t="s">
-        <v>2</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>95</v>
+        <v>146</v>
       </c>
       <c r="B76">
         <v>2</v>
       </c>
       <c r="C76">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="D76" t="s">
-        <v>96</v>
+        <v>42</v>
       </c>
       <c r="E76" t="s">
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>97</v>
+        <v>147</v>
       </c>
       <c r="B77">
         <v>2</v>
       </c>
       <c r="C77">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>98</v>
+        <v>148</v>
       </c>
       <c r="E77" t="s">
-        <v>2</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="B78">
         <v>2</v>
       </c>
       <c r="C78">
+        <v>2</v>
+      </c>
+      <c r="D78" t="s">
+        <v>43</v>
+      </c>
+      <c r="E78" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>149</v>
+      </c>
+      <c r="B79">
+        <v>2</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79" t="s">
+        <v>150</v>
+      </c>
+      <c r="E79" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>151</v>
+      </c>
+      <c r="B80">
+        <v>1</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80" t="s">
+        <v>152</v>
+      </c>
+      <c r="E80" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>153</v>
+      </c>
+      <c r="B81">
+        <v>2</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81" t="s">
+        <v>154</v>
+      </c>
+      <c r="E81" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>155</v>
+      </c>
+      <c r="B82">
+        <v>2</v>
+      </c>
+      <c r="C82">
         <v>2.5</v>
       </c>
-      <c r="D78" t="s">
-        <v>98</v>
-      </c>
-      <c r="E78" t="s">
-        <v>2</v>
+      <c r="D82" t="s">
+        <v>156</v>
+      </c>
+      <c r="E82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>155</v>
+      </c>
+      <c r="B83">
+        <v>2</v>
+      </c>
+      <c r="C83">
+        <v>2.5</v>
+      </c>
+      <c r="D83" t="s">
+        <v>22</v>
+      </c>
+      <c r="E83" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>157</v>
+      </c>
+      <c r="B84">
+        <v>3</v>
+      </c>
+      <c r="C84">
+        <v>2.5</v>
+      </c>
+      <c r="D84" t="s">
+        <v>158</v>
+      </c>
+      <c r="E84" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>159</v>
+      </c>
+      <c r="B85">
+        <v>3</v>
+      </c>
+      <c r="C85">
+        <v>2.5</v>
+      </c>
+      <c r="D85" t="s">
+        <v>160</v>
+      </c>
+      <c r="E85" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>161</v>
+      </c>
+      <c r="B86">
+        <v>3</v>
+      </c>
+      <c r="C86">
+        <v>3</v>
+      </c>
+      <c r="D86" t="s">
+        <v>162</v>
+      </c>
+      <c r="E86" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>161</v>
+      </c>
+      <c r="B87">
+        <v>3</v>
+      </c>
+      <c r="C87">
+        <v>2.5</v>
+      </c>
+      <c r="D87" t="s">
+        <v>163</v>
+      </c>
+      <c r="E87" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>161</v>
+      </c>
+      <c r="B88">
+        <v>3</v>
+      </c>
+      <c r="C88">
+        <v>2</v>
+      </c>
+      <c r="D88" t="s">
+        <v>163</v>
+      </c>
+      <c r="E88" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>164</v>
+      </c>
+      <c r="B89">
+        <v>2</v>
+      </c>
+      <c r="C89">
+        <v>3</v>
+      </c>
+      <c r="D89" t="s">
+        <v>165</v>
+      </c>
+      <c r="E89" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>166</v>
+      </c>
+      <c r="B90">
+        <v>3</v>
+      </c>
+      <c r="C90">
+        <v>2.5</v>
+      </c>
+      <c r="D90" t="s">
+        <v>167</v>
+      </c>
+      <c r="E90" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>168</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>25</v>
+      </c>
+      <c r="E91" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>170</v>
+      </c>
+      <c r="B92">
+        <v>1</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92" t="s">
+        <v>75</v>
+      </c>
+      <c r="E92" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>